<commit_message>
Gráficos dinámicos en tablas dinámica
</commit_message>
<xml_diff>
--- a/Excel/Práctica/13. Tablas Dinámicas en Excel/Introducción a tablas dinámicas.xlsx
+++ b/Excel/Práctica/13. Tablas Dinámicas en Excel/Introducción a tablas dinámicas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="4"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja5" sheetId="9" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="82">
   <si>
     <t>Etiquetas de fila</t>
   </si>
@@ -1123,6 +1123,106 @@
   <si>
     <t>Bono (10%)</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Al igual, usted también puede insertar</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> gráficos dinámicos a sus tablas dinámicas. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Primeramente hacemos click sobre la tabla dinámica en cuestión y nos vamos a la pestaña </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Insertar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, luego click en el gráfico de su interés o en la opción de </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gráficos recomendados</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Ahora, se habla de </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Gráficos dinámicos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>porque es sensible a cualquier cambio que sufra la tabla dinámica en cuestión; es decir, se actualiza el gráfico, en tiempo real, a cualquier cambio que sufra la tabla dinámica.</t>
+    </r>
+  </si>
+  <si>
+    <t>Para ver al detalle la información de cada registro sólo haga doble click sobre el registro de su interés y podrá visualizar toda la información relacionada a ese sólo registro, bajo las condiciones establecidas en la propia tabla dinámica, en una nueva tabla reflejada en una nueva hoja de cálculo. Haga el intento para entender mejor con un ejemplo.</t>
+  </si>
 </sst>
 </file>
 
@@ -1416,7 +1516,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -1466,11 +1566,21 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1478,15 +1588,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1497,7 +1600,16 @@
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="5"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -2175,7 +2287,7 @@
         </groupItems>
       </fieldGroup>
     </cacheField>
-    <cacheField name="Bono" numFmtId="0" formula="IF('Importe Venta' &gt;1500,'Importe Venta'*10%,0)" databaseField="0"/>
+    <cacheField name="Bono" numFmtId="0" formula="IF('Importe Venta'&gt;1500,'Importe Venta'*10%,0)" databaseField="0"/>
     <cacheField name="Trimestres" numFmtId="0" databaseField="0">
       <fieldGroup base="4">
         <rangePr groupBy="quarters" startDate="2020-01-03T00:00:00" endDate="2020-12-30T00:00:00"/>
@@ -3548,7 +3660,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C32" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -3737,7 +3849,7 @@
     <dataField name="Suma de Bono" fld="5" baseField="0" baseItem="0" numFmtId="44"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="3">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -3754,7 +3866,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D255" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -4628,7 +4740,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E31" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisPage" showAll="0">
@@ -4860,10 +4972,10 @@
     <dataField name="Bono (10%)" fld="5" baseField="0" baseItem="0" numFmtId="44"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="2">
+    <format dxfId="5">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -4874,7 +4986,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="3">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -4901,7 +5013,7 @@
     <tableColumn id="2" name="Vendedor"/>
     <tableColumn id="3" name="Importe Venta"/>
     <tableColumn id="4" name="Impuesto"/>
-    <tableColumn id="5" name="Mes Venta" dataDxfId="4"/>
+    <tableColumn id="5" name="Mes Venta" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9192,8 +9304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R193"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection sqref="A1:E193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -9241,14 +9353,14 @@
       <c r="G2" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -9267,12 +9379,12 @@
       <c r="E3" s="16">
         <v>43834</v>
       </c>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
     </row>
     <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -9291,12 +9403,12 @@
       <c r="E4" s="12">
         <v>44077</v>
       </c>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
     </row>
     <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -9315,12 +9427,12 @@
       <c r="E5" s="16">
         <v>43860</v>
       </c>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
     </row>
     <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -9357,14 +9469,14 @@
       <c r="E7" s="16">
         <v>44087</v>
       </c>
-      <c r="M7" s="35" t="s">
+      <c r="M7" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="36"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
     </row>
     <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
@@ -9383,12 +9495,12 @@
       <c r="E8" s="12">
         <v>44094</v>
       </c>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="36"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
     </row>
     <row r="9" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -9407,12 +9519,12 @@
       <c r="E9" s="16">
         <v>44076</v>
       </c>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="36"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
     </row>
     <row r="10" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -9431,12 +9543,12 @@
       <c r="E10" s="12">
         <v>44107</v>
       </c>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="36"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
     </row>
     <row r="11" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -9473,14 +9585,14 @@
       <c r="E12" s="12">
         <v>44174</v>
       </c>
-      <c r="M12" s="35" t="s">
+      <c r="M12" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
     </row>
     <row r="13" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -9499,12 +9611,12 @@
       <c r="E13" s="16">
         <v>44097</v>
       </c>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
     </row>
     <row r="14" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -9523,12 +9635,12 @@
       <c r="E14" s="12">
         <v>44045</v>
       </c>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
     </row>
     <row r="15" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
@@ -9547,12 +9659,12 @@
       <c r="E15" s="16">
         <v>44073</v>
       </c>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
     </row>
     <row r="16" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -9571,12 +9683,12 @@
       <c r="E16" s="12">
         <v>43884</v>
       </c>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
     </row>
     <row r="17" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -9595,12 +9707,12 @@
       <c r="E17" s="16">
         <v>43934</v>
       </c>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
     </row>
     <row r="18" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
@@ -9619,12 +9731,12 @@
       <c r="E18" s="12">
         <v>43920</v>
       </c>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
     </row>
     <row r="19" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
@@ -9643,12 +9755,12 @@
       <c r="E19" s="16">
         <v>44094</v>
       </c>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="35"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
     </row>
     <row r="20" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -12818,10 +12930,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -12862,14 +12974,14 @@
       <c r="E3" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -12887,12 +12999,12 @@
       <c r="E4" s="33">
         <v>1310</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -12910,12 +13022,12 @@
       <c r="E5" s="33">
         <v>870</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -12933,12 +13045,12 @@
       <c r="E6" s="33">
         <v>870</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -12956,12 +13068,12 @@
       <c r="E7" s="33">
         <v>1400</v>
       </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -12996,7 +13108,7 @@
       <c r="E9" s="33">
         <v>590</v>
       </c>
-      <c r="G9" s="40" t="s">
+      <c r="G9" s="36" t="s">
         <v>68</v>
       </c>
     </row>
@@ -13033,14 +13145,14 @@
       <c r="E11" s="33">
         <v>460</v>
       </c>
-      <c r="G11" s="38" t="s">
+      <c r="G11" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -13058,12 +13170,12 @@
       <c r="E12" s="33">
         <v>400</v>
       </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -13322,14 +13434,14 @@
       <c r="E27" s="33">
         <v>0</v>
       </c>
-      <c r="G27" s="38" t="s">
+      <c r="G27" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -13347,12 +13459,12 @@
       <c r="E28" s="33">
         <v>0</v>
       </c>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
@@ -13405,118 +13517,146 @@
         <v>21410</v>
       </c>
     </row>
-    <row r="36" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G36" s="37" t="s">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="39"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="39"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="39"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="G36" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="37"/>
-      <c r="L36" s="37"/>
-    </row>
-    <row r="37" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="37"/>
-      <c r="L37" s="37"/>
-    </row>
-    <row r="38" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="37"/>
-      <c r="L38" s="37"/>
-    </row>
-    <row r="39" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-    </row>
-    <row r="41" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="41"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G37" s="41"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
+      <c r="K37" s="41"/>
+      <c r="L37" s="41"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
+      <c r="K38" s="41"/>
+      <c r="L38" s="41"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G39" s="41"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="41"/>
+      <c r="L39" s="41"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I41" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="7:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G43" s="37" t="s">
+    <row r="43" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G43" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="H43" s="37"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="37"/>
-      <c r="K43" s="37"/>
-      <c r="L43" s="37"/>
-    </row>
-    <row r="44" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="37"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="37"/>
-      <c r="L44" s="37"/>
-    </row>
-    <row r="45" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G45" s="37"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37"/>
-      <c r="K45" s="37"/>
-      <c r="L45" s="37"/>
-    </row>
-    <row r="46" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G46" s="37"/>
-      <c r="H46" s="37"/>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="37"/>
-      <c r="L46" s="37"/>
-    </row>
-    <row r="47" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G47" s="37"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
-      <c r="K47" s="37"/>
-      <c r="L47" s="37"/>
-    </row>
-    <row r="48" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G48" s="37"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="37"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="37"/>
-      <c r="L48" s="37"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
+      <c r="K43" s="41"/>
+      <c r="L43" s="41"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G44" s="41"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
+      <c r="K44" s="41"/>
+      <c r="L44" s="41"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G45" s="41"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
+      <c r="K45" s="41"/>
+      <c r="L45" s="41"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="41"/>
+      <c r="L46" s="41"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="41"/>
+      <c r="K47" s="41"/>
+      <c r="L47" s="41"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G48" s="41"/>
+      <c r="H48" s="41"/>
+      <c r="I48" s="41"/>
+      <c r="J48" s="41"/>
+      <c r="K48" s="41"/>
+      <c r="L48" s="41"/>
     </row>
     <row r="49" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G49" s="37"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="37"/>
-      <c r="J49" s="37"/>
-      <c r="K49" s="37"/>
-      <c r="L49" s="37"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="41"/>
+      <c r="J49" s="41"/>
+      <c r="K49" s="41"/>
+      <c r="L49" s="41"/>
     </row>
     <row r="50" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="37"/>
-      <c r="J50" s="37"/>
-      <c r="K50" s="37"/>
-      <c r="L50" s="37"/>
+      <c r="G50" s="41"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="41"/>
+      <c r="J50" s="41"/>
+      <c r="K50" s="41"/>
+      <c r="L50" s="41"/>
     </row>
     <row r="51" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G51" s="37"/>
-      <c r="H51" s="37"/>
-      <c r="I51" s="37"/>
-      <c r="J51" s="37"/>
-      <c r="K51" s="37"/>
-      <c r="L51" s="37"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="41"/>
+      <c r="J51" s="41"/>
+      <c r="K51" s="41"/>
+      <c r="L51" s="41"/>
     </row>
     <row r="53" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
@@ -13529,54 +13669,54 @@
       </c>
     </row>
     <row r="56" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G56" s="35" t="s">
+      <c r="G56" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="H56" s="35"/>
-      <c r="I56" s="35"/>
-      <c r="J56" s="35"/>
-      <c r="K56" s="35"/>
-      <c r="L56" s="35"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37"/>
+      <c r="L56" s="37"/>
     </row>
     <row r="57" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G57" s="35"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="35"/>
-      <c r="K57" s="35"/>
-      <c r="L57" s="35"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="37"/>
     </row>
     <row r="58" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G58" s="35"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="35"/>
-      <c r="K58" s="35"/>
-      <c r="L58" s="35"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="37"/>
+      <c r="L58" s="37"/>
     </row>
     <row r="59" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G59" s="35"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="35"/>
-      <c r="J59" s="35"/>
-      <c r="K59" s="35"/>
-      <c r="L59" s="35"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="37"/>
+      <c r="L59" s="37"/>
     </row>
     <row r="60" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G60" s="35"/>
-      <c r="H60" s="35"/>
-      <c r="I60" s="35"/>
-      <c r="J60" s="35"/>
-      <c r="K60" s="35"/>
-      <c r="L60" s="35"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="37"/>
+      <c r="K60" s="37"/>
+      <c r="L60" s="37"/>
     </row>
     <row r="61" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G61" s="35"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="35"/>
-      <c r="J61" s="35"/>
-      <c r="K61" s="35"/>
-      <c r="L61" s="35"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="37"/>
+      <c r="K61" s="37"/>
+      <c r="L61" s="37"/>
     </row>
     <row r="71" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G71" s="29" t="s">
@@ -13584,54 +13724,54 @@
       </c>
     </row>
     <row r="73" spans="7:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J73" s="37" t="s">
+      <c r="J73" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="K73" s="37"/>
-      <c r="L73" s="37"/>
-      <c r="M73" s="37"/>
+      <c r="K73" s="41"/>
+      <c r="L73" s="41"/>
+      <c r="M73" s="41"/>
     </row>
     <row r="74" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J74" s="37"/>
-      <c r="K74" s="37"/>
-      <c r="L74" s="37"/>
-      <c r="M74" s="37"/>
+      <c r="J74" s="41"/>
+      <c r="K74" s="41"/>
+      <c r="L74" s="41"/>
+      <c r="M74" s="41"/>
     </row>
     <row r="75" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J75" s="37"/>
-      <c r="K75" s="37"/>
-      <c r="L75" s="37"/>
-      <c r="M75" s="37"/>
+      <c r="J75" s="41"/>
+      <c r="K75" s="41"/>
+      <c r="L75" s="41"/>
+      <c r="M75" s="41"/>
     </row>
     <row r="76" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J76" s="37"/>
-      <c r="K76" s="37"/>
-      <c r="L76" s="37"/>
-      <c r="M76" s="37"/>
+      <c r="J76" s="41"/>
+      <c r="K76" s="41"/>
+      <c r="L76" s="41"/>
+      <c r="M76" s="41"/>
     </row>
     <row r="77" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J77" s="37"/>
-      <c r="K77" s="37"/>
-      <c r="L77" s="37"/>
-      <c r="M77" s="37"/>
+      <c r="J77" s="41"/>
+      <c r="K77" s="41"/>
+      <c r="L77" s="41"/>
+      <c r="M77" s="41"/>
     </row>
     <row r="78" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J78" s="37"/>
-      <c r="K78" s="37"/>
-      <c r="L78" s="37"/>
-      <c r="M78" s="37"/>
+      <c r="J78" s="41"/>
+      <c r="K78" s="41"/>
+      <c r="L78" s="41"/>
+      <c r="M78" s="41"/>
     </row>
     <row r="79" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J79" s="37"/>
-      <c r="K79" s="37"/>
-      <c r="L79" s="37"/>
-      <c r="M79" s="37"/>
+      <c r="J79" s="41"/>
+      <c r="K79" s="41"/>
+      <c r="L79" s="41"/>
+      <c r="M79" s="41"/>
     </row>
     <row r="80" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J80" s="39"/>
-      <c r="K80" s="39"/>
-      <c r="L80" s="39"/>
-      <c r="M80" s="39"/>
+      <c r="J80" s="35"/>
+      <c r="K80" s="35"/>
+      <c r="L80" s="35"/>
+      <c r="M80" s="35"/>
     </row>
     <row r="81" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G81" s="29" t="s">
@@ -13639,103 +13779,139 @@
       </c>
     </row>
     <row r="82" spans="7:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J82" s="37" t="s">
+      <c r="J82" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="K82" s="37"/>
-      <c r="L82" s="37"/>
-      <c r="M82" s="37"/>
+      <c r="K82" s="41"/>
+      <c r="L82" s="41"/>
+      <c r="M82" s="41"/>
     </row>
     <row r="83" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J83" s="37"/>
-      <c r="K83" s="37"/>
-      <c r="L83" s="37"/>
-      <c r="M83" s="37"/>
+      <c r="J83" s="41"/>
+      <c r="K83" s="41"/>
+      <c r="L83" s="41"/>
+      <c r="M83" s="41"/>
     </row>
     <row r="84" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J84" s="37"/>
-      <c r="K84" s="37"/>
-      <c r="L84" s="37"/>
-      <c r="M84" s="37"/>
+      <c r="J84" s="41"/>
+      <c r="K84" s="41"/>
+      <c r="L84" s="41"/>
+      <c r="M84" s="41"/>
     </row>
     <row r="85" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J85" s="37"/>
-      <c r="K85" s="37"/>
-      <c r="L85" s="37"/>
-      <c r="M85" s="37"/>
+      <c r="J85" s="41"/>
+      <c r="K85" s="41"/>
+      <c r="L85" s="41"/>
+      <c r="M85" s="41"/>
     </row>
     <row r="86" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J86" s="37"/>
-      <c r="K86" s="37"/>
-      <c r="L86" s="37"/>
-      <c r="M86" s="37"/>
+      <c r="J86" s="41"/>
+      <c r="K86" s="41"/>
+      <c r="L86" s="41"/>
+      <c r="M86" s="41"/>
     </row>
     <row r="87" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J87" s="37"/>
-      <c r="K87" s="37"/>
-      <c r="L87" s="37"/>
-      <c r="M87" s="37"/>
+      <c r="J87" s="41"/>
+      <c r="K87" s="41"/>
+      <c r="L87" s="41"/>
+      <c r="M87" s="41"/>
     </row>
     <row r="88" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J88" s="37"/>
-      <c r="K88" s="37"/>
-      <c r="L88" s="37"/>
-      <c r="M88" s="37"/>
+      <c r="J88" s="41"/>
+      <c r="K88" s="41"/>
+      <c r="L88" s="41"/>
+      <c r="M88" s="41"/>
     </row>
     <row r="89" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J89" s="37"/>
-      <c r="K89" s="37"/>
-      <c r="L89" s="37"/>
-      <c r="M89" s="37"/>
+      <c r="J89" s="41"/>
+      <c r="K89" s="41"/>
+      <c r="L89" s="41"/>
+      <c r="M89" s="41"/>
     </row>
     <row r="90" spans="7:13" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G90" s="42" t="s">
+      <c r="G90" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="H90" s="42"/>
-      <c r="J90" s="37"/>
-      <c r="K90" s="37"/>
-      <c r="L90" s="37"/>
-      <c r="M90" s="37"/>
+      <c r="H90" s="40"/>
+      <c r="J90" s="41"/>
+      <c r="K90" s="41"/>
+      <c r="L90" s="41"/>
+      <c r="M90" s="41"/>
     </row>
     <row r="91" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G91" s="42"/>
-      <c r="H91" s="42"/>
-      <c r="J91" s="37"/>
-      <c r="K91" s="37"/>
-      <c r="L91" s="37"/>
-      <c r="M91" s="37"/>
+      <c r="G91" s="40"/>
+      <c r="H91" s="40"/>
+      <c r="J91" s="41"/>
+      <c r="K91" s="41"/>
+      <c r="L91" s="41"/>
+      <c r="M91" s="41"/>
     </row>
     <row r="92" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G92" s="39"/>
-      <c r="H92" s="39"/>
+      <c r="G92" s="35"/>
+      <c r="H92" s="35"/>
     </row>
     <row r="93" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J93" s="41" t="s">
+      <c r="J93" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="K93" s="41"/>
-      <c r="L93" s="41"/>
-      <c r="M93" s="41"/>
+      <c r="K93" s="39"/>
+      <c r="L93" s="39"/>
+      <c r="M93" s="39"/>
     </row>
     <row r="94" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="J94" s="41"/>
-      <c r="K94" s="41"/>
-      <c r="L94" s="41"/>
-      <c r="M94" s="41"/>
+      <c r="J94" s="39"/>
+      <c r="K94" s="39"/>
+      <c r="L94" s="39"/>
+      <c r="M94" s="39"/>
+    </row>
+    <row r="96" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G96" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="H96" s="43"/>
+      <c r="I96" s="43"/>
+      <c r="J96" s="43"/>
+      <c r="K96" s="43"/>
+      <c r="L96" s="43"/>
+    </row>
+    <row r="97" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G97" s="43"/>
+      <c r="H97" s="43"/>
+      <c r="I97" s="43"/>
+      <c r="J97" s="43"/>
+      <c r="K97" s="43"/>
+      <c r="L97" s="43"/>
+    </row>
+    <row r="98" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G98" s="43"/>
+      <c r="H98" s="43"/>
+      <c r="I98" s="43"/>
+      <c r="J98" s="43"/>
+      <c r="K98" s="43"/>
+      <c r="L98" s="43"/>
+    </row>
+    <row r="99" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G99" s="43"/>
+      <c r="H99" s="43"/>
+      <c r="I99" s="43"/>
+      <c r="J99" s="43"/>
+      <c r="K99" s="43"/>
+      <c r="L99" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="G96:L99"/>
+    <mergeCell ref="A33:E36"/>
+    <mergeCell ref="G3:L7"/>
+    <mergeCell ref="G11:L12"/>
+    <mergeCell ref="G27:L28"/>
+    <mergeCell ref="G36:L39"/>
+    <mergeCell ref="G43:L51"/>
     <mergeCell ref="J93:M94"/>
     <mergeCell ref="G90:H91"/>
     <mergeCell ref="G56:L61"/>
     <mergeCell ref="J73:M79"/>
     <mergeCell ref="J82:M91"/>
-    <mergeCell ref="G3:L7"/>
-    <mergeCell ref="G11:L12"/>
-    <mergeCell ref="G27:L28"/>
-    <mergeCell ref="G36:L39"/>
-    <mergeCell ref="G43:L51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>

</xml_diff>